<commit_message>
fix gp.Number related issues
</commit_message>
<xml_diff>
--- a/models/cta/results.xlsx
+++ b/models/cta/results.xlsx
@@ -4121,19 +4121,19 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>194.999948143959</v>
+        <v>108.0001937225461</v>
       </c>
       <c r="E17" t="n">
-        <v>175.9998500347137</v>
+        <v>123.0002380907536</v>
       </c>
       <c r="F17" t="n">
-        <v>148.9996444433928</v>
+        <v>115.0001306086779</v>
       </c>
       <c r="G17" t="n">
-        <v>169.0005417913198</v>
+        <v>130.0001749768853</v>
       </c>
       <c r="H17" t="n">
-        <v>214.0000462532043</v>
+        <v>125.9994925931096</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
update heatex and inscribedsquare
</commit_message>
<xml_diff>
--- a/models/cta/results.xlsx
+++ b/models/cta/results.xlsx
@@ -4121,19 +4121,19 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>108.0001937225461</v>
+        <v>220.9999831393361</v>
       </c>
       <c r="E17" t="n">
-        <v>123.0002380907536</v>
+        <v>157.9999225214124</v>
       </c>
       <c r="F17" t="n">
-        <v>115.0001306086779</v>
+        <v>185.9996700659394</v>
       </c>
       <c r="G17" t="n">
-        <v>130.0001749768853</v>
+        <v>216.0003874450922</v>
       </c>
       <c r="H17" t="n">
-        <v>125.9994925931096</v>
+        <v>152.9996981844306</v>
       </c>
     </row>
     <row r="18">

</xml_diff>